<commit_message>
Add unit test for structure file errors in scenario 14
</commit_message>
<xml_diff>
--- a/input_data/data_errors_14/proporcionalidades.xlsx
+++ b/input_data/data_errors_14/proporcionalidades.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="20">
   <si>
     <t xml:space="preserve">2-2015</t>
   </si>
@@ -43,6 +43,9 @@
     <t xml:space="preserve">6-2015</t>
   </si>
   <si>
+    <t xml:space="preserve">:8-2015</t>
+  </si>
+  <si>
     <t xml:space="preserve">id</t>
   </si>
   <si>
@@ -71,6 +74,9 @@
   </si>
   <si>
     <t xml:space="preserve">9-2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">:9-2015</t>
   </si>
   <si>
     <t xml:space="preserve">DI</t>
@@ -303,10 +309,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:X6"/>
+  <dimension ref="A1:Z6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="R1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U13" activeCellId="0" sqref="U13"/>
+      <selection pane="topLeft" activeCell="Z2" activeCellId="0" sqref="Z2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.34375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -354,79 +360,88 @@
         <v>6</v>
       </c>
       <c r="X1" s="2"/>
+      <c r="Y1" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="U2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -446,7 +461,7 @@
         <v>0.442</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G3" s="1" t="n">
         <v>0.558</v>
@@ -500,6 +515,12 @@
         <v>0.442</v>
       </c>
       <c r="X3" s="1" t="n">
+        <v>0.558</v>
+      </c>
+      <c r="Y3" s="1" t="n">
+        <v>0.442</v>
+      </c>
+      <c r="Z3" s="1" t="n">
         <v>0.558</v>
       </c>
     </row>
@@ -520,7 +541,7 @@
         <v>0.442</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G4" s="1" t="n">
         <v>0.558</v>
@@ -574,6 +595,12 @@
         <v>0.442</v>
       </c>
       <c r="X4" s="1" t="n">
+        <v>0.558</v>
+      </c>
+      <c r="Y4" s="1" t="n">
+        <v>0.442</v>
+      </c>
+      <c r="Z4" s="1" t="n">
         <v>0.558</v>
       </c>
     </row>
@@ -594,7 +621,7 @@
         <v>0.442</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G5" s="1" t="n">
         <v>0.558</v>
@@ -648,6 +675,12 @@
         <v>0</v>
       </c>
       <c r="X5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -668,7 +701,7 @@
         <v>0.442</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G6" s="1" t="n">
         <v>0.558</v>
@@ -719,10 +752,16 @@
         <v>0.262</v>
       </c>
       <c r="W6" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="X6" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>